<commit_message>
Add new default font, make titles bold by user setting and update excel template
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wolfkain/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wolfkain/Projects/360/Apps/dualpresenter/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436EDB0F-0DD9-FA49-8CB9-B17EB4DF1567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD68E4B-12E2-7940-B291-0C57F09957E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="27300" xr2:uid="{31235C52-23CF-6F4B-906D-2BCD49615FB2}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -449,6 +449,12 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Presenter</t>
   </si>
 </sst>
 </file>
@@ -529,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -573,60 +579,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="33">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
-        <color auto="1"/>
+        <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFCAD2D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF6E684F"/>
-          <bgColor rgb="FFF1F2DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF6E684F"/>
-          <bgColor rgb="FFF1F2DA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -684,11 +655,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="1"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC5CBF2"/>
         </patternFill>
       </fill>
     </dxf>
@@ -908,19 +879,20 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="TableStyleLight8 2" pivot="0" count="9" xr9:uid="{80D2B743-4329-6544-8889-4B0B004A6420}">
-      <tableStyleElement type="wholeTable" dxfId="35"/>
-      <tableStyleElement type="headerRow" dxfId="34"/>
-      <tableStyleElement type="totalRow" dxfId="33"/>
-      <tableStyleElement type="firstColumn" dxfId="32"/>
-      <tableStyleElement type="lastColumn" dxfId="31"/>
-      <tableStyleElement type="firstRowStripe" dxfId="30"/>
-      <tableStyleElement type="secondRowStripe" dxfId="29"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="28"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="31"/>
+      <tableStyleElement type="totalRow" dxfId="30"/>
+      <tableStyleElement type="firstColumn" dxfId="29"/>
+      <tableStyleElement type="lastColumn" dxfId="28"/>
+      <tableStyleElement type="firstRowStripe" dxfId="27"/>
+      <tableStyleElement type="secondRowStripe" dxfId="26"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="25"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="24"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFC5CBF2"/>
       <color rgb="FF6E684F"/>
       <color rgb="FFF1F2DA"/>
       <color rgb="FFCEF3E1"/>
@@ -941,38 +913,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84E6271E-1140-5E4E-8C94-6B7E104C92AD}" name="Flow" displayName="Flow" ref="A1:I62" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{84E6271E-1140-5E4E-8C94-6B7E104C92AD}" name="Flow" displayName="Flow" ref="A1:I62" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A1:I62" xr:uid="{84E6271E-1140-5E4E-8C94-6B7E104C92AD}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I62">
     <sortCondition ref="A1:A62"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="10" xr3:uid="{9FB372EE-CC04-3D4B-B0DB-CDB6BC0707DC}" name="#" dataDxfId="24">
+    <tableColumn id="10" xr3:uid="{9FB372EE-CC04-3D4B-B0DB-CDB6BC0707DC}" name="#" dataDxfId="21">
       <calculatedColumnFormula>ROW()-1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D373A835-1BA4-AE45-9363-EE67E6165767}" name="Type" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{DA0621C3-BCB2-254D-93C7-AC63CC141306}" name="Title" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{57A8305B-55FC-E949-81F4-841B61FC4B23}" name="Subtitle" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{5BC695E7-5490-5647-A005-C433DAA5B19B}" name="Group" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{0C3D6887-B103-F14F-9A95-9058AB0F7C1C}" name="From" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{872D8E49-A803-AA40-AD08-83386EB17B64}" name="Until" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{6F06AFA4-A4D4-E242-AA22-F08727EA7CF0}" name="Main Only" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{7A62BBC9-6DF9-694F-A31F-9635C8DE492C}" name="Precedence" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{D373A835-1BA4-AE45-9363-EE67E6165767}" name="Type" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{DA0621C3-BCB2-254D-93C7-AC63CC141306}" name="Title" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{57A8305B-55FC-E949-81F4-841B61FC4B23}" name="Subtitle" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{5BC695E7-5490-5647-A005-C433DAA5B19B}" name="Group" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{0C3D6887-B103-F14F-9A95-9058AB0F7C1C}" name="From" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{872D8E49-A803-AA40-AD08-83386EB17B64}" name="Until" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{6F06AFA4-A4D4-E242-AA22-F08727EA7CF0}" name="Main Only" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{7A62BBC9-6DF9-694F-A31F-9635C8DE492C}" name="Precedence" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DD68603-088B-0B49-BA2F-E26D2888A5DB}" name="Names" displayName="Names" ref="A1:C73">
-  <autoFilter ref="A1:C73" xr:uid="{7DD68603-088B-0B49-BA2F-E26D2888A5DB}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DD68603-088B-0B49-BA2F-E26D2888A5DB}" name="Names" displayName="Names" ref="A1:D73">
+  <autoFilter ref="A1:D73" xr:uid="{7DD68603-088B-0B49-BA2F-E26D2888A5DB}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D73">
     <sortCondition ref="B2:B73"/>
     <sortCondition ref="A2:A73"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{54EDEFF7-6D50-644B-86D9-EB6D272BB5CB}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{1FC3351A-5F59-8344-918E-0052C96220FD}" name="Group"/>
+    <tableColumn id="4" xr3:uid="{C8E79D04-D70B-2344-B5CA-715A391DE5C9}" name="Presenter" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{DCF0A96D-147F-D842-B4A4-575507D6A1CD}" name="Attending" totalsRowFunction="count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1300,7 +1273,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,9 +1419,9 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="6"/>
@@ -1519,15 +1492,15 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="6"/>
@@ -1841,7 +1814,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>50</v>
@@ -2658,7 +2631,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>1</v>
+        <v>129</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>82</v>
@@ -6180,19 +6153,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:I62">
-    <cfRule type="expression" dxfId="15" priority="11">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
+      <formula>$B2="Category"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="12">
       <formula>$B2="Image"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="5" priority="13">
       <formula>$B2="Unattended"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="13">
+    <cfRule type="expression" dxfId="4" priority="14">
       <formula>$B2="Names"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14">
+    <cfRule type="expression" dxfId="3" priority="15">
       <formula>$B2="Title"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="2" priority="16">
       <formula>$B2="Blank"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6203,11 +6179,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G62" xr:uid="{4F7EC304-E9E0-844B-A75C-0D3F224D3A31}">
       <formula1>_xlfn.ANCHORARRAY(AA2)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B62" xr:uid="{149ED5FE-6586-D048-9D95-0A1F563EE7B0}">
-      <formula1>"Blank,Title,Names,Unattended,Image"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H62" xr:uid="{00458457-181C-DD48-B0A3-3AA4591A8F19}">
       <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{8912C3EE-AF9E-DB4D-B520-9FF14DF891AD}">
+      <formula1>"Blank,Category,Title,Names,Unattended,Image"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6238,831 +6214,835 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1937413E-4502-604B-9F19-827CE90D7D87}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="52.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34" style="15" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
       <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>86</v>
       </c>
       <c r="B5" t="s">
         <v>82</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>82</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
       <c r="B7" t="s">
         <v>82</v>
       </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>89</v>
       </c>
       <c r="B8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>90</v>
       </c>
       <c r="B9" t="s">
         <v>82</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>91</v>
       </c>
       <c r="B10" t="s">
         <v>82</v>
       </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>82</v>
       </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>95</v>
       </c>
       <c r="B12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>96</v>
       </c>
       <c r="B13" t="s">
         <v>82</v>
       </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>97</v>
       </c>
       <c r="B14" t="s">
         <v>82</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>98</v>
       </c>
       <c r="B15" t="s">
         <v>82</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>99</v>
       </c>
       <c r="B16" t="s">
         <v>82</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>100</v>
       </c>
       <c r="B17" t="s">
         <v>82</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>103</v>
       </c>
       <c r="B18" t="s">
         <v>82</v>
       </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>104</v>
       </c>
       <c r="B19" t="s">
         <v>82</v>
       </c>
-      <c r="C19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>105</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
       </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>106</v>
       </c>
       <c r="B21" t="s">
         <v>82</v>
       </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>107</v>
       </c>
       <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="C22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>82</v>
       </c>
-      <c r="C23" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>109</v>
       </c>
       <c r="B24" t="s">
         <v>82</v>
       </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>112</v>
       </c>
       <c r="B25" t="s">
         <v>82</v>
       </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>113</v>
       </c>
       <c r="B26" t="s">
         <v>82</v>
       </c>
-      <c r="C26" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>114</v>
       </c>
       <c r="B27" t="s">
         <v>82</v>
       </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>115</v>
       </c>
       <c r="B28" t="s">
         <v>82</v>
       </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>116</v>
       </c>
       <c r="B29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>117</v>
       </c>
       <c r="B30" t="s">
         <v>82</v>
       </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>124</v>
       </c>
       <c r="B31" t="s">
         <v>82</v>
       </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>118</v>
       </c>
       <c r="B32" t="s">
         <v>82</v>
       </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>125</v>
       </c>
       <c r="B33" t="s">
         <v>82</v>
       </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>126</v>
       </c>
       <c r="B34" t="s">
         <v>82</v>
       </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>127</v>
       </c>
       <c r="B35" t="s">
         <v>82</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>7</v>
       </c>
       <c r="B36" t="s">
         <v>50</v>
       </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37" t="s">
         <v>50</v>
       </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
       <c r="B38" t="s">
         <v>50</v>
       </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
         <v>50</v>
       </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>54</v>
       </c>
       <c r="B40" t="s">
         <v>50</v>
       </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>55</v>
       </c>
       <c r="B41" t="s">
         <v>50</v>
       </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>56</v>
       </c>
       <c r="B42" t="s">
         <v>50</v>
       </c>
-      <c r="C42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>57</v>
       </c>
       <c r="B43" t="s">
         <v>50</v>
       </c>
-      <c r="C43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>60</v>
       </c>
       <c r="B44" t="s">
         <v>50</v>
       </c>
-      <c r="C44" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>61</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
       </c>
-      <c r="C45" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>63</v>
       </c>
       <c r="B46" t="s">
         <v>50</v>
       </c>
-      <c r="C46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>62</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
       </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>66</v>
       </c>
       <c r="B48" t="s">
         <v>50</v>
       </c>
-      <c r="C48" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>68</v>
       </c>
       <c r="B49" t="s">
         <v>50</v>
       </c>
-      <c r="C49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>67</v>
       </c>
       <c r="B50" t="s">
         <v>50</v>
       </c>
-      <c r="C50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>69</v>
       </c>
       <c r="B51" t="s">
         <v>50</v>
       </c>
-      <c r="C51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>72</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
       </c>
-      <c r="C52" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>73</v>
       </c>
       <c r="B53" t="s">
         <v>50</v>
       </c>
-      <c r="C53" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D53" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>74</v>
       </c>
       <c r="B54" t="s">
         <v>50</v>
       </c>
-      <c r="C54" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D54" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>75</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
       </c>
-      <c r="C55" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D55" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>78</v>
       </c>
       <c r="B56" t="s">
         <v>50</v>
       </c>
-      <c r="C56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>79</v>
       </c>
       <c r="B57" t="s">
         <v>50</v>
       </c>
-      <c r="C57" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>80</v>
       </c>
       <c r="B58" t="s">
         <v>50</v>
       </c>
-      <c r="C58" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>81</v>
       </c>
       <c r="B59" t="s">
         <v>50</v>
       </c>
-      <c r="C59" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>32</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
       </c>
-      <c r="C60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>33</v>
       </c>
       <c r="B61" t="s">
         <v>11</v>
       </c>
-      <c r="C61" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>34</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
       </c>
-      <c r="C62" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>35</v>
       </c>
       <c r="B63" t="s">
         <v>11</v>
       </c>
-      <c r="C63" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>36</v>
       </c>
       <c r="B64" t="s">
         <v>11</v>
       </c>
-      <c r="C64" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>40</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
       </c>
-      <c r="C65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>41</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
       </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>42</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
       </c>
-      <c r="C67" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>43</v>
       </c>
       <c r="B68" t="s">
         <v>11</v>
       </c>
-      <c r="C68" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>46</v>
       </c>
       <c r="B69" t="s">
         <v>11</v>
       </c>
-      <c r="C69" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>47</v>
       </c>
       <c r="B70" t="s">
         <v>11</v>
       </c>
-      <c r="C70" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>49</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
       </c>
-      <c r="C71" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>48</v>
       </c>
       <c r="B72" t="s">
         <v>11</v>
       </c>
-      <c r="C72" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>27</v>
       </c>
       <c r="B73" t="s">
         <v>26</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{6A3E8714-88DE-7A4A-853D-7DAA6A3F83E2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{6A3E8714-88DE-7A4A-853D-7DAA6A3F83E2}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update templates and add client template
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wolfkain/Projects/360/Apps/dualpresenter/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wolfkain/Projects/360/Edits/2025/Empowering Youth 2025/Dualpresenter/Thriasio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E662FEE-E5B9-4A46-9A9D-6DD2AA73886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF46D594-F939-B04D-B5F2-92BFFFD94307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20580" xr2:uid="{31235C52-23CF-6F4B-906D-2BCD49615FB2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="27300" xr2:uid="{31235C52-23CF-6F4B-906D-2BCD49615FB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Flow" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,6 @@
     <t>Καράμπελας Αλέξανδρος - Παρασκευάς</t>
   </si>
   <si>
-    <t>Μέσος Όρος Βαθμολογίας +19</t>
-  </si>
-  <si>
-    <t>Μέσος Όρος Βαθμολογίας +18</t>
-  </si>
-  <si>
     <t>Ζαμπέτη Κυριακή</t>
   </si>
   <si>
@@ -222,9 +216,6 @@
     <t>Βαλτάς Δημήτριος</t>
   </si>
   <si>
-    <t>Μέσος Όρος Βαθμολογίας +17</t>
-  </si>
-  <si>
     <t>Βλαχαντώνη Γεωργία</t>
   </si>
   <si>
@@ -309,9 +300,6 @@
     <t>Χατζημηνά Αναστασία</t>
   </si>
   <si>
-    <t>Μέσος Όρος Βαθμολογίας +16</t>
-  </si>
-  <si>
     <t>Γεωργούσης Κωνσταντίνος</t>
   </si>
   <si>
@@ -372,19 +360,10 @@
     <t>Χαβαριώτης Ιωάννης</t>
   </si>
   <si>
-    <t>Μέσος Όρος βαθμολογίας +19</t>
-  </si>
-  <si>
     <t xml:space="preserve">Σοφία Ζαχαράκη </t>
   </si>
   <si>
     <t xml:space="preserve">Υπουργός Παιδείας, Θρησκευμάτων και Αθλητισμού </t>
-  </si>
-  <si>
-    <t>Μέσος Όρος βαθμολογίας +18</t>
-  </si>
-  <si>
-    <t>Μέσος Όρος βαθμολογίας +17</t>
   </si>
   <si>
     <t xml:space="preserve">Ευάγγελος Λιάκος </t>
@@ -399,9 +378,6 @@
   </si>
   <si>
     <t>Γεώργιος Γεωργόπουλος</t>
-  </si>
-  <si>
-    <t>Μέσος Όρος βαθμολογίας +16</t>
   </si>
   <si>
     <t>Περιφερειακός Σύμβουλος Δυτικής Αττικής</t>
@@ -510,6 +486,30 @@
   </si>
   <si>
     <t>Τσίγκρη Ελένη</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος Βαθμολογίας 16+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος Βαθμολογίας 17+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος Βαθμολογίας 18+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος Βαθμολογίας 19+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος βαθμολογίας 19+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος βαθμολογίας 18+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος βαθμολογίας 17+</t>
+  </si>
+  <si>
+    <t>Μέσος Όρος βαθμολογίας 16+</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -556,6 +556,12 @@
     <font>
       <sz val="11"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -628,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -679,10 +685,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1391,7 +1396,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1501,10 +1506,10 @@
         <v>15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>13</v>
@@ -1530,10 +1535,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="1"/>
@@ -1600,7 +1605,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="1"/>
@@ -1640,7 +1645,7 @@
       </c>
       <c r="C11" s="11"/>
       <c r="E11" s="2" t="s">
-        <v>42</v>
+        <v>143</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
@@ -1674,7 +1679,7 @@
         <v>40</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="1"/>
@@ -1714,13 +1719,13 @@
       </c>
       <c r="C15" s="11"/>
       <c r="E15" s="2" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="1"/>
@@ -1813,13 +1818,13 @@
       <c r="C18" s="11"/>
       <c r="D18" s="4"/>
       <c r="E18" s="2" t="s">
-        <v>43</v>
+        <v>142</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
@@ -1890,7 +1895,7 @@
         <v>40</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="D20" s="4"/>
       <c r="I20" s="6"/>
@@ -1909,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>21</v>
@@ -1932,13 +1937,13 @@
       <c r="C22" s="11"/>
       <c r="D22" s="4"/>
       <c r="E22" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="1"/>
@@ -2105,7 +2110,7 @@
         <v>33</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="1"/>
@@ -2125,13 +2130,13 @@
       <c r="C25" s="11"/>
       <c r="D25" s="4"/>
       <c r="E25" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="1"/>
@@ -2298,7 +2303,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="1"/>
@@ -2318,13 +2323,13 @@
       <c r="C28" s="11"/>
       <c r="D28" s="4"/>
       <c r="E28" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="1"/>
@@ -2511,13 +2516,13 @@
       <c r="C31" s="11"/>
       <c r="D31" s="4"/>
       <c r="E31" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="1"/>
@@ -2681,7 +2686,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>26</v>
@@ -2704,13 +2709,13 @@
       <c r="C34" s="11"/>
       <c r="D34" s="4"/>
       <c r="E34" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="1"/>
@@ -2897,13 +2902,13 @@
       <c r="C37" s="11"/>
       <c r="D37" s="4"/>
       <c r="E37" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I37" s="6"/>
       <c r="J37" s="1"/>
@@ -3090,13 +3095,13 @@
       <c r="C40" s="11"/>
       <c r="D40" s="4"/>
       <c r="E40" s="2" t="s">
-        <v>53</v>
+        <v>141</v>
       </c>
       <c r="F40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="I40" s="6"/>
       <c r="J40" s="1"/>
@@ -3260,7 +3265,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>112</v>
+        <v>147</v>
       </c>
       <c r="D42" s="4"/>
       <c r="I42" s="6"/>
@@ -3302,13 +3307,13 @@
       <c r="C44" s="11"/>
       <c r="D44" s="4"/>
       <c r="E44" s="2" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="1"/>
@@ -3427,7 +3432,7 @@
         <v>38</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="1"/>
@@ -3447,13 +3452,13 @@
       <c r="C47" s="11"/>
       <c r="D47" s="4"/>
       <c r="E47" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="I47" s="6"/>
       <c r="J47" s="1"/>
@@ -3569,10 +3574,10 @@
         <v>1</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="1"/>
@@ -3592,13 +3597,13 @@
       <c r="C50" s="11"/>
       <c r="D50" s="4"/>
       <c r="E50" s="2" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="1"/>
@@ -3717,7 +3722,7 @@
         <v>36</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="1"/>
@@ -3737,13 +3742,13 @@
       <c r="C53" s="11"/>
       <c r="D53" s="4"/>
       <c r="E53" s="2" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="F53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I53" s="6"/>
       <c r="J53" s="1"/>
@@ -3862,7 +3867,7 @@
         <v>37</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="I55" s="6"/>
       <c r="J55" s="1"/>
@@ -3882,13 +3887,13 @@
       <c r="C56" s="11"/>
       <c r="D56" s="4"/>
       <c r="E56" s="2" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="1"/>
@@ -6679,7 +6684,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6702,7 +6707,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B2" s="17" t="s">
         <v>15</v>
@@ -6724,10 +6729,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>82</v>
+        <v>133</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>6</v>
@@ -6735,10 +6740,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>82</v>
+        <v>134</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>6</v>
@@ -6746,10 +6751,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>82</v>
+        <v>79</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>6</v>
@@ -6757,10 +6762,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>82</v>
+        <v>135</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>6</v>
@@ -6768,10 +6773,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>6</v>
@@ -6779,10 +6784,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>6</v>
@@ -6790,10 +6795,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="18" t="s">
         <v>82</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>6</v>
@@ -6801,10 +6806,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C11" s="18" t="s">
         <v>6</v>
@@ -6812,10 +6817,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>6</v>
@@ -6823,21 +6828,21 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>82</v>
+      <c r="A14" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>6</v>
@@ -6845,10 +6850,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>6</v>
@@ -6856,10 +6861,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>82</v>
+        <v>136</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>6</v>
@@ -6867,10 +6872,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>6</v>
@@ -6878,10 +6883,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>82</v>
+        <v>88</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>6</v>
@@ -6889,10 +6894,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="18" t="s">
-        <v>82</v>
+        <v>89</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C19" s="18" t="s">
         <v>6</v>
@@ -6900,10 +6905,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>82</v>
+        <v>137</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C20" s="18" t="s">
         <v>6</v>
@@ -6911,10 +6916,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>82</v>
+        <v>90</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>6</v>
@@ -6922,10 +6927,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>82</v>
+        <v>91</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>6</v>
@@ -6933,10 +6938,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>82</v>
+        <v>92</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C23" s="18" t="s">
         <v>6</v>
@@ -6944,10 +6949,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>82</v>
+        <v>93</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C24" s="18" t="s">
         <v>6</v>
@@ -6955,10 +6960,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>82</v>
+        <v>94</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C25" s="18" t="s">
         <v>6</v>
@@ -6966,10 +6971,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>82</v>
+        <v>95</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C26" s="18" t="s">
         <v>6</v>
@@ -6977,10 +6982,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>82</v>
+        <v>138</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C27" s="18" t="s">
         <v>6</v>
@@ -6988,10 +6993,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B28" s="18" t="s">
-        <v>82</v>
+        <v>96</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C28" s="18" t="s">
         <v>6</v>
@@ -6999,10 +7004,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>82</v>
+        <v>139</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C29" s="18" t="s">
         <v>6</v>
@@ -7010,10 +7015,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>82</v>
+        <v>97</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>6</v>
@@ -7021,10 +7026,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="B31" s="18" t="s">
-        <v>82</v>
+        <v>98</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>140</v>
       </c>
       <c r="C31" s="18" t="s">
         <v>6</v>
@@ -7032,10 +7037,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>6</v>
@@ -7043,10 +7048,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>53</v>
+        <v>51</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C33" s="18" t="s">
         <v>6</v>
@@ -7054,10 +7059,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C34" s="18" t="s">
         <v>6</v>
@@ -7065,10 +7070,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>53</v>
+        <v>118</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C35" s="18" t="s">
         <v>6</v>
@@ -7076,10 +7081,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="18" t="s">
         <v>53</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C36" s="18" t="s">
         <v>6</v>
@@ -7087,10 +7092,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="B37" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C37" s="18" t="s">
         <v>6</v>
@@ -7098,10 +7103,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>6</v>
@@ -7109,10 +7114,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>53</v>
+        <v>119</v>
+      </c>
+      <c r="B39" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C39" s="18" t="s">
         <v>6</v>
@@ -7120,10 +7125,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>53</v>
+        <v>120</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C40" s="18" t="s">
         <v>6</v>
@@ -7131,10 +7136,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B41" s="18" t="s">
-        <v>53</v>
+        <v>121</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C41" s="18" t="s">
         <v>6</v>
@@ -7142,10 +7147,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>53</v>
+        <v>122</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C42" s="18" t="s">
         <v>6</v>
@@ -7153,10 +7158,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="18" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>6</v>
@@ -7164,10 +7169,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>53</v>
+        <v>57</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C44" s="18" t="s">
         <v>6</v>
@@ -7175,10 +7180,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="18" t="s">
-        <v>53</v>
+        <v>123</v>
+      </c>
+      <c r="B45" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C45" s="18" t="s">
         <v>6</v>
@@ -7186,10 +7191,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="18" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C46" s="18" t="s">
         <v>6</v>
@@ -7197,10 +7202,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B47" s="18" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C47" s="18" t="s">
         <v>6</v>
@@ -7208,10 +7213,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>53</v>
+        <v>60</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C48" s="18" t="s">
         <v>6</v>
@@ -7219,10 +7224,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="B49" s="18" t="s">
-        <v>53</v>
+        <v>61</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C49" s="18" t="s">
         <v>6</v>
@@ -7230,10 +7235,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B50" s="18" t="s">
-        <v>53</v>
+        <v>62</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>6</v>
@@ -7241,10 +7246,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" s="18" t="s">
-        <v>53</v>
+        <v>124</v>
+      </c>
+      <c r="B51" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C51" s="18" t="s">
         <v>6</v>
@@ -7252,10 +7257,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B52" s="18" t="s">
-        <v>53</v>
+        <v>63</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C52" s="18" t="s">
         <v>6</v>
@@ -7263,10 +7268,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B53" s="18" t="s">
-        <v>53</v>
+        <v>64</v>
+      </c>
+      <c r="B53" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C53" s="18" t="s">
         <v>6</v>
@@ -7274,10 +7279,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B54" s="18" t="s">
-        <v>53</v>
+        <v>65</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C54" s="18" t="s">
         <v>6</v>
@@ -7285,10 +7290,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="B55" s="18" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="B55" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C55" s="18" t="s">
         <v>6</v>
@@ -7296,21 +7301,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="B56" s="18" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C56" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="21" t="s">
-        <v>133</v>
-      </c>
-      <c r="B57" s="18" t="s">
-        <v>53</v>
+      <c r="A57" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C57" s="18" t="s">
         <v>6</v>
@@ -7318,10 +7323,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="B58" s="18" t="s">
-        <v>53</v>
+        <v>68</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C58" s="18" t="s">
         <v>6</v>
@@ -7329,10 +7334,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B59" s="18" t="s">
-        <v>53</v>
+        <v>69</v>
+      </c>
+      <c r="B59" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C59" s="18" t="s">
         <v>6</v>
@@ -7340,10 +7345,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>53</v>
+        <v>70</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>6</v>
@@ -7351,10 +7356,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>53</v>
+        <v>126</v>
+      </c>
+      <c r="B61" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C61" s="18" t="s">
         <v>6</v>
@@ -7362,10 +7367,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="18" t="s">
-        <v>53</v>
+        <v>71</v>
+      </c>
+      <c r="B62" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C62" s="18" t="s">
         <v>6</v>
@@ -7373,10 +7378,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B63" s="18" t="s">
-        <v>53</v>
+        <v>72</v>
+      </c>
+      <c r="B63" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C63" s="18" t="s">
         <v>6</v>
@@ -7384,10 +7389,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B64" s="18" t="s">
-        <v>53</v>
+        <v>127</v>
+      </c>
+      <c r="B64" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C64" s="18" t="s">
         <v>6</v>
@@ -7395,10 +7400,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
-        <v>136</v>
-      </c>
-      <c r="B65" s="18" t="s">
-        <v>53</v>
+        <v>128</v>
+      </c>
+      <c r="B65" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>6</v>
@@ -7406,10 +7411,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="B66" s="18" t="s">
-        <v>53</v>
+        <v>129</v>
+      </c>
+      <c r="B66" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C66" s="18" t="s">
         <v>6</v>
@@ -7417,10 +7422,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="B67" s="18" t="s">
-        <v>53</v>
+        <v>73</v>
+      </c>
+      <c r="B67" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>6</v>
@@ -7428,10 +7433,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B68" s="18" t="s">
-        <v>53</v>
+        <v>74</v>
+      </c>
+      <c r="B68" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>6</v>
@@ -7439,10 +7444,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>53</v>
+        <v>75</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>6</v>
@@ -7450,10 +7455,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B70" s="20" t="s">
-        <v>53</v>
+        <v>76</v>
+      </c>
+      <c r="B70" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>6</v>
@@ -7461,10 +7466,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B71" s="20" t="s">
-        <v>53</v>
+        <v>130</v>
+      </c>
+      <c r="B71" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C71" s="18" t="s">
         <v>6</v>
@@ -7472,10 +7477,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="20" t="s">
-        <v>53</v>
+        <v>77</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C72" s="18" t="s">
         <v>6</v>
@@ -7483,10 +7488,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B73" s="20" t="s">
-        <v>53</v>
+        <v>131</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C73" s="18" t="s">
         <v>6</v>
@@ -7494,10 +7499,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="20" t="s">
-        <v>53</v>
+        <v>132</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C74" s="18" t="s">
         <v>6</v>
@@ -7505,21 +7510,21 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75" s="20" t="s">
-        <v>53</v>
+        <v>78</v>
+      </c>
+      <c r="B75" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="C75" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="B76" s="18" t="s">
-        <v>43</v>
+      <c r="A76" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C76" s="18" t="s">
         <v>6</v>
@@ -7527,21 +7532,21 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B77" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C77" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B78" s="18" t="s">
-        <v>43</v>
+      <c r="A78" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C78" s="18" t="s">
         <v>6</v>
@@ -7549,10 +7554,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="B79" s="18" t="s">
-        <v>43</v>
+        <v>115</v>
+      </c>
+      <c r="B79" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C79" s="18" t="s">
         <v>6</v>
@@ -7560,10 +7565,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B80" s="18" t="s">
         <v>43</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C80" s="18" t="s">
         <v>6</v>
@@ -7571,10 +7576,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B81" s="18" t="s">
-        <v>43</v>
+        <v>116</v>
+      </c>
+      <c r="B81" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C81" s="18" t="s">
         <v>6</v>
@@ -7582,10 +7587,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B82" s="18" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="B82" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C82" s="18" t="s">
         <v>6</v>
@@ -7593,10 +7598,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="B83" s="18" t="s">
-        <v>43</v>
+        <v>117</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C83" s="18" t="s">
         <v>6</v>
@@ -7604,10 +7609,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B84" s="18" t="s">
-        <v>43</v>
+        <v>45</v>
+      </c>
+      <c r="B84" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C84" s="18" t="s">
         <v>6</v>
@@ -7615,10 +7620,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B85" s="18" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="B85" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C85" s="18" t="s">
         <v>6</v>
@@ -7626,10 +7631,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B86" s="18" t="s">
-        <v>43</v>
+        <v>47</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C86" s="18" t="s">
         <v>6</v>
@@ -7637,10 +7642,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B87" s="18" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="B87" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C87" s="18" t="s">
         <v>6</v>
@@ -7648,21 +7653,21 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B88" s="18" t="s">
-        <v>43</v>
+        <v>49</v>
+      </c>
+      <c r="B88" s="22" t="s">
+        <v>142</v>
       </c>
       <c r="C88" s="18" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="21" t="s">
-        <v>119</v>
-      </c>
-      <c r="B89" s="18" t="s">
-        <v>42</v>
+      <c r="A89" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B89" s="22" t="s">
+        <v>143</v>
       </c>
       <c r="C89" s="18" t="s">
         <v>6</v>
@@ -7674,7 +7679,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{6A3E8714-88DE-7A4A-853D-7DAA6A3F83E2}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>

</xml_diff>